<commit_message>
Test using and import
</commit_message>
<xml_diff>
--- a/src/test-haxe/com/qifun/qforce/importCsv/TestConfig.xlsx
+++ b/src/test-haxe/com/qifun/qforce/importCsv/TestConfig.xlsx
@@ -10,6 +10,8 @@
     <sheet name="Foo" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="import" sheetId="4" r:id="rId4"/>
+    <sheet name="using" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
   <webPublishing codePage="65001"/>
@@ -17,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>"中文"</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -164,6 +166,29 @@
   </si>
   <si>
     <t>xx=$xx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StringTools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ttt.startsWith("")?1:2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.qifun.qforce.importCsv.StringInterpolation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>haxe.ds.Option</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switch (None) {
+case None: 1;
+case Some(v): 2;
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +612,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -677,9 +702,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="135">
       <c r="A10" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -714,7 +742,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -793,6 +821,9 @@
         <v>28</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -817,4 +848,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>